<commit_message>
progress of the day
- cleaned and formatted all the datasets
- merged marketing_actions with dates
- developed aditional features for marketing_actions per dates for model training and further analysis
- created aditional KPIs useful for modeling team
</commit_message>
<xml_diff>
--- a/Data/Original/Dates.xlsx
+++ b/Data/Original/Dates.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\aaSmartQuest\Ediciones SM\Abandono\Datathon\Ficheros finales\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pma/Documents/GitHub/DATATHON_2/Data/Original/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3686075B-2CC2-4A74-9717-41E10452C288}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81587251-265C-214B-A960-7B13486E0C91}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{09F34DE4-81DF-4196-8693-C499AB825130}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="23260" windowHeight="12720" xr2:uid="{09F34DE4-81DF-4196-8693-C499AB825130}"/>
   </bookViews>
   <sheets>
     <sheet name="dates" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">dates!$A$1:$F$10</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -33,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="12">
   <si>
     <t>Course Year</t>
   </si>
@@ -76,7 +79,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="[$-409]mmm\-yy;@"/>
+    <numFmt numFmtId="164" formatCode="[$-409]mmm\-yy;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -134,7 +137,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -449,65 +452,65 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D6B4287-79E6-49E9-B9FA-C9F52053A154}">
-  <dimension ref="A1:AX13"/>
+  <dimension ref="A1:AX10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="6" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C7" sqref="C7"/>
+      <selection pane="bottomRight" activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.1640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.5546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.83203125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="7" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.77734375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="6.5546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="6.77734375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="6.5" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="7.1640625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="6.5546875" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="5.83203125" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="7" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="6.77734375" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="6.5546875" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="6.77734375" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="6.5" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="7.1640625" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="6.5546875" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="5.83203125" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="7" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="6.77734375" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="6.5546875" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="6.77734375" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="6.5" bestFit="1" customWidth="1"/>
     <col min="44" max="44" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="7.1640625" bestFit="1" customWidth="1"/>
     <col min="46" max="46" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="6.5546875" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="5.83203125" bestFit="1" customWidth="1"/>
     <col min="50" max="50" width="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:50" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:50" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -659,7 +662,7 @@
         <v>44044</v>
       </c>
     </row>
-    <row r="2" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -691,7 +694,7 @@
       <c r="AT2" s="3"/>
       <c r="AU2" s="3"/>
     </row>
-    <row r="3" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -723,7 +726,7 @@
       <c r="AO3" s="3"/>
       <c r="AP3" s="3"/>
     </row>
-    <row r="4" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -756,191 +759,192 @@
       <c r="AT4" s="3"/>
       <c r="AU4" s="3"/>
     </row>
-    <row r="5" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="2">
-        <v>43709</v>
+        <v>43282</v>
       </c>
       <c r="D5" s="2">
-        <v>43799</v>
+        <v>43373</v>
       </c>
       <c r="E5" s="2">
-        <v>43709</v>
+        <v>43252</v>
       </c>
       <c r="F5" s="2">
-        <v>44075</v>
-      </c>
-      <c r="AM5" s="4"/>
-      <c r="AN5" s="4"/>
-      <c r="AO5" s="4"/>
-      <c r="AP5" s="3"/>
-      <c r="AQ5" s="3"/>
-      <c r="AR5" s="3"/>
-      <c r="AS5" s="3"/>
-      <c r="AT5" s="3"/>
-      <c r="AU5" s="3"/>
-      <c r="AV5" s="3"/>
-      <c r="AW5" s="3"/>
-      <c r="AX5" s="3"/>
+        <v>43617</v>
+      </c>
+      <c r="X5" s="3"/>
+      <c r="Y5" s="4"/>
+      <c r="Z5" s="4"/>
+      <c r="AA5" s="4"/>
+      <c r="AB5" s="3"/>
+      <c r="AC5" s="3"/>
+      <c r="AD5" s="3"/>
+      <c r="AE5" s="3"/>
+      <c r="AF5" s="3"/>
+      <c r="AG5" s="3"/>
+      <c r="AH5" s="3"/>
+      <c r="AI5" s="3"/>
     </row>
-    <row r="6" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C6" s="2">
-        <v>43282</v>
+        <v>43101</v>
       </c>
       <c r="D6" s="2">
-        <v>43373</v>
+        <v>43220</v>
       </c>
       <c r="E6" s="2">
-        <v>43252</v>
+        <v>43101</v>
       </c>
       <c r="F6" s="2">
-        <v>43617</v>
-      </c>
+        <v>43466</v>
+      </c>
+      <c r="S6" s="4"/>
+      <c r="T6" s="4"/>
+      <c r="U6" s="4"/>
+      <c r="V6" s="4"/>
+      <c r="W6" s="3"/>
       <c r="X6" s="3"/>
-      <c r="Y6" s="4"/>
-      <c r="Z6" s="4"/>
-      <c r="AA6" s="4"/>
+      <c r="Y6" s="3"/>
+      <c r="Z6" s="3"/>
+      <c r="AA6" s="3"/>
       <c r="AB6" s="3"/>
       <c r="AC6" s="3"/>
       <c r="AD6" s="3"/>
-      <c r="AE6" s="3"/>
-      <c r="AF6" s="3"/>
-      <c r="AG6" s="3"/>
-      <c r="AH6" s="3"/>
-      <c r="AI6" s="3"/>
     </row>
-    <row r="7" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C7" s="2">
-        <v>43101</v>
+        <v>43337</v>
       </c>
       <c r="D7" s="2">
-        <v>43220</v>
+        <v>43434</v>
       </c>
       <c r="E7" s="2">
-        <v>43101</v>
+        <v>43235</v>
       </c>
       <c r="F7" s="2">
-        <v>43466</v>
-      </c>
-      <c r="S7" s="4"/>
-      <c r="T7" s="4"/>
-      <c r="U7" s="4"/>
-      <c r="V7" s="4"/>
+        <v>43600</v>
+      </c>
       <c r="W7" s="3"/>
       <c r="X7" s="3"/>
       <c r="Y7" s="3"/>
       <c r="Z7" s="3"/>
-      <c r="AA7" s="3"/>
-      <c r="AB7" s="3"/>
+      <c r="AA7" s="4"/>
+      <c r="AB7" s="4"/>
       <c r="AC7" s="3"/>
       <c r="AD7" s="3"/>
+      <c r="AE7" s="3"/>
+      <c r="AF7" s="3"/>
+      <c r="AG7" s="3"/>
+      <c r="AH7" s="3"/>
+      <c r="AI7" s="3"/>
     </row>
-    <row r="8" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C8" s="2">
-        <v>43337</v>
+        <v>42917</v>
       </c>
       <c r="D8" s="2">
-        <v>43434</v>
+        <v>43008</v>
       </c>
       <c r="E8" s="2">
-        <v>43235</v>
+        <v>42887</v>
       </c>
       <c r="F8" s="2">
-        <v>43600</v>
-      </c>
+        <v>43252</v>
+      </c>
+      <c r="L8" s="3"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="4"/>
+      <c r="O8" s="4"/>
+      <c r="P8" s="3"/>
+      <c r="Q8" s="3"/>
+      <c r="R8" s="3"/>
+      <c r="S8" s="3"/>
+      <c r="T8" s="3"/>
+      <c r="U8" s="3"/>
+      <c r="V8" s="3"/>
       <c r="W8" s="3"/>
-      <c r="X8" s="3"/>
-      <c r="Y8" s="3"/>
-      <c r="Z8" s="3"/>
-      <c r="AA8" s="4"/>
-      <c r="AB8" s="4"/>
-      <c r="AC8" s="3"/>
-      <c r="AD8" s="3"/>
-      <c r="AE8" s="3"/>
-      <c r="AF8" s="3"/>
-      <c r="AG8" s="3"/>
-      <c r="AH8" s="3"/>
-      <c r="AI8" s="3"/>
     </row>
-    <row r="9" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C9" s="2">
-        <v>43344</v>
+        <v>42736</v>
       </c>
       <c r="D9" s="2">
-        <v>43434</v>
+        <v>42855</v>
       </c>
       <c r="E9" s="2">
-        <v>43344</v>
+        <v>42736</v>
       </c>
       <c r="F9" s="2">
-        <v>43709</v>
-      </c>
-      <c r="AA9" s="4"/>
-      <c r="AB9" s="4"/>
-      <c r="AC9" s="4"/>
-      <c r="AD9" s="3"/>
-      <c r="AE9" s="3"/>
-      <c r="AF9" s="3"/>
-      <c r="AG9" s="3"/>
-      <c r="AH9" s="3"/>
-      <c r="AI9" s="3"/>
-      <c r="AJ9" s="3"/>
-      <c r="AK9" s="3"/>
-      <c r="AL9" s="3"/>
+        <v>43101</v>
+      </c>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
+      <c r="P9" s="3"/>
+      <c r="Q9" s="3"/>
+      <c r="R9" s="3"/>
     </row>
-    <row r="10" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B10" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C10" s="2">
-        <v>42917</v>
+        <v>42972</v>
       </c>
       <c r="D10" s="2">
-        <v>43008</v>
+        <v>43069</v>
       </c>
       <c r="E10" s="2">
-        <v>42887</v>
+        <v>42870</v>
       </c>
       <c r="F10" s="2">
-        <v>43252</v>
-      </c>
+        <v>43235</v>
+      </c>
+      <c r="K10" s="3"/>
       <c r="L10" s="3"/>
-      <c r="M10" s="4"/>
-      <c r="N10" s="4"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
       <c r="O10" s="4"/>
-      <c r="P10" s="3"/>
+      <c r="P10" s="4"/>
       <c r="Q10" s="3"/>
       <c r="R10" s="3"/>
       <c r="S10" s="3"/>
@@ -949,104 +953,8 @@
       <c r="V10" s="3"/>
       <c r="W10" s="3"/>
     </row>
-    <row r="11" spans="1:50" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" s="2">
-        <v>42736</v>
-      </c>
-      <c r="D11" s="2">
-        <v>42855</v>
-      </c>
-      <c r="E11" s="2">
-        <v>42736</v>
-      </c>
-      <c r="F11" s="2">
-        <v>43101</v>
-      </c>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="4"/>
-      <c r="K11" s="3"/>
-      <c r="L11" s="3"/>
-      <c r="M11" s="3"/>
-      <c r="N11" s="3"/>
-      <c r="O11" s="3"/>
-      <c r="P11" s="3"/>
-      <c r="Q11" s="3"/>
-      <c r="R11" s="3"/>
-    </row>
-    <row r="12" spans="1:50" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B12" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" s="2">
-        <v>42972</v>
-      </c>
-      <c r="D12" s="2">
-        <v>43069</v>
-      </c>
-      <c r="E12" s="2">
-        <v>42870</v>
-      </c>
-      <c r="F12" s="2">
-        <v>43235</v>
-      </c>
-      <c r="K12" s="3"/>
-      <c r="L12" s="3"/>
-      <c r="M12" s="3"/>
-      <c r="N12" s="3"/>
-      <c r="O12" s="4"/>
-      <c r="P12" s="4"/>
-      <c r="Q12" s="3"/>
-      <c r="R12" s="3"/>
-      <c r="S12" s="3"/>
-      <c r="T12" s="3"/>
-      <c r="U12" s="3"/>
-      <c r="V12" s="3"/>
-      <c r="W12" s="3"/>
-    </row>
-    <row r="13" spans="1:50" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" s="2">
-        <v>42979</v>
-      </c>
-      <c r="D13" s="2">
-        <v>43069</v>
-      </c>
-      <c r="E13" s="2">
-        <v>42979</v>
-      </c>
-      <c r="F13" s="2">
-        <v>43344</v>
-      </c>
-      <c r="O13" s="4"/>
-      <c r="P13" s="4"/>
-      <c r="Q13" s="4"/>
-      <c r="R13" s="3"/>
-      <c r="S13" s="3"/>
-      <c r="T13" s="3"/>
-      <c r="U13" s="3"/>
-      <c r="V13" s="3"/>
-      <c r="W13" s="3"/>
-      <c r="X13" s="3"/>
-      <c r="Y13" s="3"/>
-      <c r="Z13" s="3"/>
-    </row>
   </sheetData>
+  <autoFilter ref="A1:F10" xr:uid="{D33E9BE3-8A0D-D14C-89F6-44E01716C012}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>